<commit_message>
Updates to Script For Figure Creation - Gough
</commit_message>
<xml_diff>
--- a/Finalized Data Sheet For Hayden.xlsx
+++ b/Finalized Data Sheet For Hayden.xlsx
@@ -14,12 +14,15 @@
   <sheets>
     <sheet name="Finalized Data Sheet For Hayden" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="114">
+  <si>
+    <t>IDNum</t>
+  </si>
   <si>
     <t>Whale</t>
   </si>
@@ -27,12 +30,72 @@
     <t>Species</t>
   </si>
   <si>
+    <t>TotLength</t>
+  </si>
+  <si>
+    <t>Log10TotLength</t>
+  </si>
+  <si>
+    <t>MassPerLength</t>
+  </si>
+  <si>
+    <t>MassFromTL</t>
+  </si>
+  <si>
     <t>Log Mass</t>
   </si>
   <si>
+    <t>SA Coeff</t>
+  </si>
+  <si>
+    <t>SurfArea</t>
+  </si>
+  <si>
+    <t>FlukeArea</t>
+  </si>
+  <si>
     <t>FA/L</t>
   </si>
   <si>
+    <t>ChordLength</t>
+  </si>
+  <si>
+    <t>MaxDiam</t>
+  </si>
+  <si>
+    <t>FinenessRatio</t>
+  </si>
+  <si>
+    <t>RunGenOrIndividual</t>
+  </si>
+  <si>
+    <t>w_max/TL</t>
+  </si>
+  <si>
+    <t>pressure drag coef 2nd bracket</t>
+  </si>
+  <si>
+    <t>friction drag 1st bracket</t>
+  </si>
+  <si>
+    <t>Drag force (N)</t>
+  </si>
+  <si>
+    <t>rho</t>
+  </si>
+  <si>
+    <t>nu</t>
+  </si>
+  <si>
+    <t>F_twidle</t>
+  </si>
+  <si>
+    <t>speed U</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
     <t>Special Notes</t>
   </si>
   <si>
@@ -42,9 +105,18 @@
     <t>Minke</t>
   </si>
   <si>
+    <t>General</t>
+  </si>
+  <si>
     <t>bb180304-45</t>
   </si>
   <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>Speed messed up near end. Removed A series of flukebeats without speed (7360-end).</t>
+  </si>
+  <si>
     <t>bp170907-41b</t>
   </si>
   <si>
@@ -114,6 +186,9 @@
     <t>bw180904-48</t>
   </si>
   <si>
+    <t>Use Aw(:,1)</t>
+  </si>
+  <si>
     <t>bw180905-53</t>
   </si>
   <si>
@@ -210,6 +285,9 @@
     <t>mn180302-47</t>
   </si>
   <si>
+    <t>No completed lunge file.</t>
+  </si>
+  <si>
     <t>mn180831-11</t>
   </si>
   <si>
@@ -279,55 +357,10 @@
     <t>bs190322-49</t>
   </si>
   <si>
-    <t>TotLength</t>
-  </si>
-  <si>
-    <t>IDNum</t>
-  </si>
-  <si>
-    <t>Log10TotLength</t>
-  </si>
-  <si>
-    <t>MassFromTL</t>
-  </si>
-  <si>
-    <t>MassPerLength</t>
-  </si>
-  <si>
-    <t>SA Coeff</t>
-  </si>
-  <si>
-    <t>SurfArea</t>
-  </si>
-  <si>
-    <t>FlukeArea</t>
-  </si>
-  <si>
-    <t>ChordLength</t>
-  </si>
-  <si>
-    <t>MaxDiam</t>
-  </si>
-  <si>
-    <t>FinenessRatio</t>
-  </si>
-  <si>
-    <t>Use Aw(:,1)</t>
-  </si>
-  <si>
-    <t>General</t>
-  </si>
-  <si>
-    <t>Individual</t>
-  </si>
-  <si>
-    <t>RunGenOrIndividual</t>
-  </si>
-  <si>
-    <t>Speed messed up near end. Removed A series of flukebeats without speed (7360-end).</t>
-  </si>
-  <si>
-    <t>No completed lunge file.</t>
+    <t>drag coefficient C_D Model</t>
+  </si>
+  <si>
+    <t>Reynolds Number Model</t>
   </si>
 </sst>
 </file>
@@ -811,10 +844,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1136,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q70"/>
+  <dimension ref="A1:AB70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1154,72 +1185,116 @@
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
     <col min="12" max="14" width="12" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" customWidth="1"/>
-    <col min="17" max="17" width="62.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="72.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>90</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>94</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>95</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>113</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>112</v>
+      </c>
+      <c r="V1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D2">
         <v>8.0394576559999997</v>
@@ -1258,18 +1333,51 @@
         <v>5.6442808539999998</v>
       </c>
       <c r="P2" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q2">
+        <v>0.17717048899999999</v>
+      </c>
+      <c r="R2">
+        <v>1.150789812</v>
+      </c>
+      <c r="S2">
+        <v>13511693.539999999</v>
+      </c>
+      <c r="T2">
+        <v>2.6989230000000002E-3</v>
+      </c>
+      <c r="U2">
+        <v>3.1058930000000002E-3</v>
+      </c>
+      <c r="V2">
+        <v>179.15758729999999</v>
+      </c>
+      <c r="W2">
+        <v>1025</v>
+      </c>
+      <c r="X2">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>2</v>
+      </c>
+      <c r="AA2">
+        <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D3">
         <v>8.6209207879999994</v>
@@ -1308,21 +1416,54 @@
         <v>5.9701104779999996</v>
       </c>
       <c r="P3" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>101</v>
+        <v>30</v>
+      </c>
+      <c r="Q3">
+        <v>0.16750108799999999</v>
+      </c>
+      <c r="R3">
+        <v>1.1357260899999999</v>
+      </c>
+      <c r="S3">
+        <v>14488942.5</v>
+      </c>
+      <c r="T3">
+        <v>2.6614920000000001E-3</v>
+      </c>
+      <c r="U3">
+        <v>3.0227259999999999E-3</v>
+      </c>
+      <c r="V3">
+        <v>186.97103039999999</v>
+      </c>
+      <c r="W3">
+        <v>1025</v>
+      </c>
+      <c r="X3">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>2</v>
+      </c>
+      <c r="AA3">
+        <v>2050</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D4">
         <v>18.47</v>
@@ -1355,21 +1496,54 @@
         <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>10</v>
+        <v>30</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>31042016.809999999</v>
+      </c>
+      <c r="T4">
+        <v>2.285296E-3</v>
+      </c>
+      <c r="U4">
+        <v>2.285296E-3</v>
+      </c>
+      <c r="V4">
+        <v>503.16531800000001</v>
+      </c>
+      <c r="W4">
+        <v>1025</v>
+      </c>
+      <c r="X4">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4">
+        <v>2</v>
+      </c>
+      <c r="AA4">
+        <v>2050</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>19.329999999999998</v>
@@ -1408,18 +1582,51 @@
         <v>10.173684209999999</v>
       </c>
       <c r="P5" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q5">
+        <v>9.8292808999999995E-2</v>
+      </c>
+      <c r="R5">
+        <v>1.052872252</v>
+      </c>
+      <c r="S5">
+        <v>32487394.960000001</v>
+      </c>
+      <c r="T5">
+        <v>2.2645899999999999E-3</v>
+      </c>
+      <c r="U5">
+        <v>2.3843240000000002E-3</v>
+      </c>
+      <c r="V5">
+        <v>549.41225880000002</v>
+      </c>
+      <c r="W5">
+        <v>1025</v>
+      </c>
+      <c r="X5">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>2</v>
+      </c>
+      <c r="AA5">
+        <v>2050</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D6">
         <v>22.59</v>
@@ -1452,21 +1659,54 @@
         <v>1.33</v>
       </c>
       <c r="P6" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>14</v>
+        <v>28</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>37966386.549999997</v>
+      </c>
+      <c r="T6">
+        <v>2.1950920000000001E-3</v>
+      </c>
+      <c r="U6">
+        <v>2.1950920000000001E-3</v>
+      </c>
+      <c r="V6">
+        <v>688.88651100000004</v>
+      </c>
+      <c r="W6">
+        <v>1025</v>
+      </c>
+      <c r="X6">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>2</v>
+      </c>
+      <c r="AA6">
+        <v>2050</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D7">
         <v>22.21</v>
@@ -1505,18 +1745,51 @@
         <v>8.1955719560000002</v>
       </c>
       <c r="P7" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q7">
+        <v>0.122017109</v>
+      </c>
+      <c r="R7">
+        <v>1.0766488830000001</v>
+      </c>
+      <c r="S7">
+        <v>37327731.090000004</v>
+      </c>
+      <c r="T7">
+        <v>2.202552E-3</v>
+      </c>
+      <c r="U7">
+        <v>2.3713749999999998E-3</v>
+      </c>
+      <c r="V7">
+        <v>731.69087249999995</v>
+      </c>
+      <c r="W7">
+        <v>1025</v>
+      </c>
+      <c r="X7">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>2</v>
+      </c>
+      <c r="AA7">
+        <v>2050</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D8">
         <v>22.53</v>
@@ -1555,18 +1828,51 @@
         <v>7.8684503379999997</v>
       </c>
       <c r="P8" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q8">
+        <v>0.12708982799999999</v>
+      </c>
+      <c r="R8">
+        <v>1.082329766</v>
+      </c>
+      <c r="S8">
+        <v>37865546.219999999</v>
+      </c>
+      <c r="T8">
+        <v>2.1962589999999999E-3</v>
+      </c>
+      <c r="U8">
+        <v>2.377077E-3</v>
+      </c>
+      <c r="V8">
+        <v>744.01767410000002</v>
+      </c>
+      <c r="W8">
+        <v>1025</v>
+      </c>
+      <c r="X8">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>2</v>
+      </c>
+      <c r="AA8">
+        <v>2050</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D9">
         <v>22.75</v>
@@ -1605,18 +1911,51 @@
         <v>7.1745283960000004</v>
       </c>
       <c r="P9" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q9">
+        <v>0.13938198399999999</v>
+      </c>
+      <c r="R9">
+        <v>1.0970098340000001</v>
+      </c>
+      <c r="S9">
+        <v>38235294.119999997</v>
+      </c>
+      <c r="T9">
+        <v>2.191995E-3</v>
+      </c>
+      <c r="U9">
+        <v>2.40464E-3</v>
+      </c>
+      <c r="V9">
+        <v>759.99430510000002</v>
+      </c>
+      <c r="W9">
+        <v>1025</v>
+      </c>
+      <c r="X9">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <v>2</v>
+      </c>
+      <c r="AA9">
+        <v>2050</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D10">
         <v>20.7</v>
@@ -1649,18 +1988,51 @@
         <v>1.04</v>
       </c>
       <c r="P10" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>34789915.969999999</v>
+      </c>
+      <c r="T10">
+        <v>2.2337870000000001E-3</v>
+      </c>
+      <c r="U10">
+        <v>2.2337870000000001E-3</v>
+      </c>
+      <c r="V10">
+        <v>642.37846430000002</v>
+      </c>
+      <c r="W10">
+        <v>1025</v>
+      </c>
+      <c r="X10">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <v>2</v>
+      </c>
+      <c r="AA10">
+        <v>2050</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D11">
         <v>22.55</v>
@@ -1699,18 +2071,51 @@
         <v>8.4591594069999996</v>
       </c>
       <c r="P11" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q11">
+        <v>0.118215056</v>
+      </c>
+      <c r="R11">
+        <v>1.0725320110000001</v>
+      </c>
+      <c r="S11">
+        <v>37899159.659999996</v>
+      </c>
+      <c r="T11">
+        <v>2.1958699999999999E-3</v>
+      </c>
+      <c r="U11">
+        <v>2.3551409999999998E-3</v>
+      </c>
+      <c r="V11">
+        <v>737.80602339999996</v>
+      </c>
+      <c r="W11">
+        <v>1025</v>
+      </c>
+      <c r="X11">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="Z11">
+        <v>2</v>
+      </c>
+      <c r="AA11">
+        <v>2050</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D12">
         <v>21.09</v>
@@ -1749,18 +2154,51 @@
         <v>8.2564975080000007</v>
       </c>
       <c r="P12" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q12">
+        <v>0.121116732</v>
+      </c>
+      <c r="R12">
+        <v>1.07566311</v>
+      </c>
+      <c r="S12">
+        <v>35445378.149999999</v>
+      </c>
+      <c r="T12">
+        <v>2.2254639999999999E-3</v>
+      </c>
+      <c r="U12">
+        <v>2.3938499999999999E-3</v>
+      </c>
+      <c r="V12">
+        <v>701.37815460000002</v>
+      </c>
+      <c r="W12">
+        <v>1025</v>
+      </c>
+      <c r="X12">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+      <c r="Z12">
+        <v>2</v>
+      </c>
+      <c r="AA12">
+        <v>2050</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D13">
         <v>21.98</v>
@@ -1799,18 +2237,51 @@
         <v>8.0051470079999998</v>
       </c>
       <c r="P13" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q13">
+        <v>0.12491963</v>
+      </c>
+      <c r="R13">
+        <v>1.079872857</v>
+      </c>
+      <c r="S13">
+        <v>36941176.469999999</v>
+      </c>
+      <c r="T13">
+        <v>2.207142E-3</v>
+      </c>
+      <c r="U13">
+        <v>2.3834329999999999E-3</v>
+      </c>
+      <c r="V13">
+        <v>727.79567780000002</v>
+      </c>
+      <c r="W13">
+        <v>1025</v>
+      </c>
+      <c r="X13">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y13">
+        <v>1</v>
+      </c>
+      <c r="Z13">
+        <v>2</v>
+      </c>
+      <c r="AA13">
+        <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D14">
         <v>22.51</v>
@@ -1849,18 +2320,51 @@
         <v>7.2612903229999999</v>
       </c>
       <c r="P14" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q14">
+        <v>0.13771657000000001</v>
+      </c>
+      <c r="R14">
+        <v>1.0949436939999999</v>
+      </c>
+      <c r="S14">
+        <v>37831932.770000003</v>
+      </c>
+      <c r="T14">
+        <v>2.1966500000000001E-3</v>
+      </c>
+      <c r="U14">
+        <v>2.4052079999999998E-3</v>
+      </c>
+      <c r="V14">
+        <v>752.15418990000001</v>
+      </c>
+      <c r="W14">
+        <v>1025</v>
+      </c>
+      <c r="X14">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="Z14">
+        <v>2</v>
+      </c>
+      <c r="AA14">
+        <v>2050</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D15">
         <v>24.12</v>
@@ -1899,18 +2403,51 @@
         <v>8.3089639940000009</v>
       </c>
       <c r="P15" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q15">
+        <v>0.120351948</v>
+      </c>
+      <c r="R15">
+        <v>1.074831088</v>
+      </c>
+      <c r="S15">
+        <v>40537815.130000003</v>
+      </c>
+      <c r="T15">
+        <v>2.1665090000000001E-3</v>
+      </c>
+      <c r="U15">
+        <v>2.3286309999999998E-3</v>
+      </c>
+      <c r="V15">
+        <v>780.2912887</v>
+      </c>
+      <c r="W15">
+        <v>1025</v>
+      </c>
+      <c r="X15">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="Z15">
+        <v>2</v>
+      </c>
+      <c r="AA15">
+        <v>2050</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D16">
         <v>21.77</v>
@@ -1949,18 +2486,51 @@
         <v>8.1255744110000006</v>
       </c>
       <c r="P16" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q16">
+        <v>0.123068223</v>
+      </c>
+      <c r="R16">
+        <v>1.0778082499999999</v>
+      </c>
+      <c r="S16">
+        <v>36588235.289999999</v>
+      </c>
+      <c r="T16">
+        <v>2.2113839999999998E-3</v>
+      </c>
+      <c r="U16">
+        <v>2.3834479999999998E-3</v>
+      </c>
+      <c r="V16">
+        <v>720.84674719999998</v>
+      </c>
+      <c r="W16">
+        <v>1025</v>
+      </c>
+      <c r="X16">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y16">
+        <v>1</v>
+      </c>
+      <c r="Z16">
+        <v>2</v>
+      </c>
+      <c r="AA16">
+        <v>2050</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D17">
         <v>22.93</v>
@@ -1999,18 +2569,51 @@
         <v>7.8692040710000004</v>
       </c>
       <c r="P17" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q17">
+        <v>0.12707765500000001</v>
+      </c>
+      <c r="R17">
+        <v>1.0823158740000001</v>
+      </c>
+      <c r="S17">
+        <v>38537815.130000003</v>
+      </c>
+      <c r="T17">
+        <v>2.1885429999999998E-3</v>
+      </c>
+      <c r="U17">
+        <v>2.3686950000000001E-3</v>
+      </c>
+      <c r="V17">
+        <v>754.55685349999999</v>
+      </c>
+      <c r="W17">
+        <v>1025</v>
+      </c>
+      <c r="X17">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y17">
+        <v>1</v>
+      </c>
+      <c r="Z17">
+        <v>2</v>
+      </c>
+      <c r="AA17">
+        <v>2050</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D18">
         <v>23.59</v>
@@ -2049,18 +2652,51 @@
         <v>6.8575581400000001</v>
       </c>
       <c r="P18" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q18">
+        <v>0.14582450199999999</v>
+      </c>
+      <c r="R18">
+        <v>1.105235435</v>
+      </c>
+      <c r="S18">
+        <v>39647058.82</v>
+      </c>
+      <c r="T18">
+        <v>2.1761570000000002E-3</v>
+      </c>
+      <c r="U18">
+        <v>2.4051659999999998E-3</v>
+      </c>
+      <c r="V18">
+        <v>788.22798460000001</v>
+      </c>
+      <c r="W18">
+        <v>1025</v>
+      </c>
+      <c r="X18">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18">
+        <v>2</v>
+      </c>
+      <c r="AA18">
+        <v>2050</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D19">
         <v>19.27</v>
@@ -2099,18 +2735,51 @@
         <v>7.9958506219999999</v>
       </c>
       <c r="P19" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q19">
+        <v>0.125064868</v>
+      </c>
+      <c r="R19">
+        <v>1.08003604</v>
+      </c>
+      <c r="S19">
+        <v>32386554.620000001</v>
+      </c>
+      <c r="T19">
+        <v>2.265998E-3</v>
+      </c>
+      <c r="U19">
+        <v>2.44736E-3</v>
+      </c>
+      <c r="V19">
+        <v>655.17650649999996</v>
+      </c>
+      <c r="W19">
+        <v>1025</v>
+      </c>
+      <c r="X19">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y19">
+        <v>1</v>
+      </c>
+      <c r="Z19">
+        <v>2</v>
+      </c>
+      <c r="AA19">
+        <v>2050</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D20">
         <v>21.98</v>
@@ -2149,18 +2818,51 @@
         <v>8.1107011070000006</v>
       </c>
       <c r="P20" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q20">
+        <v>0.123293904</v>
+      </c>
+      <c r="R20">
+        <v>1.078058379</v>
+      </c>
+      <c r="S20">
+        <v>36941176.469999999</v>
+      </c>
+      <c r="T20">
+        <v>2.207142E-3</v>
+      </c>
+      <c r="U20">
+        <v>2.3794279999999998E-3</v>
+      </c>
+      <c r="V20">
+        <v>726.57278440000005</v>
+      </c>
+      <c r="W20">
+        <v>1025</v>
+      </c>
+      <c r="X20">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
+      <c r="Z20">
+        <v>2</v>
+      </c>
+      <c r="AA20">
+        <v>2050</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D21">
         <v>25.18</v>
@@ -2199,18 +2901,51 @@
         <v>8.7430555559999998</v>
       </c>
       <c r="P21" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q21">
+        <v>0.114376489</v>
+      </c>
+      <c r="R21">
+        <v>1.068496393</v>
+      </c>
+      <c r="S21">
+        <v>42319327.729999997</v>
+      </c>
+      <c r="T21">
+        <v>2.1479530000000002E-3</v>
+      </c>
+      <c r="U21">
+        <v>2.2950800000000001E-3</v>
+      </c>
+      <c r="V21">
+        <v>802.84616519999997</v>
+      </c>
+      <c r="W21">
+        <v>1025</v>
+      </c>
+      <c r="X21">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y21">
+        <v>1</v>
+      </c>
+      <c r="Z21">
+        <v>2</v>
+      </c>
+      <c r="AA21">
+        <v>2050</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D22">
         <v>22.83</v>
@@ -2249,21 +2984,54 @@
         <v>8.1827956989999997</v>
       </c>
       <c r="P22" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>97</v>
+        <v>30</v>
+      </c>
+      <c r="Q22">
+        <v>0.122207622</v>
+      </c>
+      <c r="R22">
+        <v>1.0768583309999999</v>
+      </c>
+      <c r="S22">
+        <v>38369747.899999999</v>
+      </c>
+      <c r="T22">
+        <v>2.1904569999999998E-3</v>
+      </c>
+      <c r="U22">
+        <v>2.3588120000000001E-3</v>
+      </c>
+      <c r="V22">
+        <v>748.13159789999997</v>
+      </c>
+      <c r="W22">
+        <v>1025</v>
+      </c>
+      <c r="X22">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y22">
+        <v>1</v>
+      </c>
+      <c r="Z22">
+        <v>2</v>
+      </c>
+      <c r="AA22">
+        <v>2050</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D23">
         <v>24.49</v>
@@ -2302,18 +3070,51 @@
         <v>8.7153024909999992</v>
       </c>
       <c r="P23" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q23">
+        <v>0.11474071</v>
+      </c>
+      <c r="R23">
+        <v>1.0688741429999999</v>
+      </c>
+      <c r="S23">
+        <v>41159663.869999997</v>
+      </c>
+      <c r="T23">
+        <v>2.1599219999999999E-3</v>
+      </c>
+      <c r="U23">
+        <v>2.308685E-3</v>
+      </c>
+      <c r="V23">
+        <v>785.47487120000005</v>
+      </c>
+      <c r="W23">
+        <v>1025</v>
+      </c>
+      <c r="X23">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y23">
+        <v>1</v>
+      </c>
+      <c r="Z23">
+        <v>2</v>
+      </c>
+      <c r="AA23">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>98</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>98</v>
-      </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D24">
         <v>10.1</v>
@@ -2346,21 +3147,54 @@
         <v>0.94</v>
       </c>
       <c r="P24" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <v>16974789.920000002</v>
+      </c>
+      <c r="T24">
+        <v>2.5785270000000002E-3</v>
+      </c>
+      <c r="U24">
+        <v>2.5785270000000002E-3</v>
+      </c>
+      <c r="V24">
+        <v>296.20082780000001</v>
+      </c>
+      <c r="W24">
+        <v>1025</v>
+      </c>
+      <c r="X24">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y24">
+        <v>1</v>
+      </c>
+      <c r="Z24">
+        <v>2</v>
+      </c>
+      <c r="AA24">
+        <v>2050</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>99</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D25">
         <v>10.44</v>
@@ -2399,18 +3233,51 @@
         <v>5.3731959099999997</v>
       </c>
       <c r="P25" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q25">
+        <v>0.18610897800000001</v>
+      </c>
+      <c r="R25">
+        <v>1.1655553089999999</v>
+      </c>
+      <c r="S25">
+        <v>17546218.489999998</v>
+      </c>
+      <c r="T25">
+        <v>2.5615080000000001E-3</v>
+      </c>
+      <c r="U25">
+        <v>2.9855799999999998E-3</v>
+      </c>
+      <c r="V25">
+        <v>354.50507329999999</v>
+      </c>
+      <c r="W25">
+        <v>1025</v>
+      </c>
+      <c r="X25">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y25">
+        <v>1</v>
+      </c>
+      <c r="Z25">
+        <v>2</v>
+      </c>
+      <c r="AA25">
+        <v>2050</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>100</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D26">
         <v>12.17</v>
@@ -2449,18 +3316,51 @@
         <v>5.5748651970000003</v>
       </c>
       <c r="P26" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q26">
+        <v>0.179376535</v>
+      </c>
+      <c r="R26">
+        <v>1.15435792</v>
+      </c>
+      <c r="S26">
+        <v>20453781.510000002</v>
+      </c>
+      <c r="T26">
+        <v>2.4841500000000001E-3</v>
+      </c>
+      <c r="U26">
+        <v>2.8675979999999998E-3</v>
+      </c>
+      <c r="V26">
+        <v>396.91921000000002</v>
+      </c>
+      <c r="W26">
+        <v>1025</v>
+      </c>
+      <c r="X26">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y26">
+        <v>1</v>
+      </c>
+      <c r="Z26">
+        <v>2</v>
+      </c>
+      <c r="AA26">
+        <v>2050</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>101</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D27">
         <v>8.2200000000000006</v>
@@ -2499,18 +3399,51 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="P27" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q27">
+        <v>0.22749391699999999</v>
+      </c>
+      <c r="R27">
+        <v>1.245174566</v>
+      </c>
+      <c r="S27">
+        <v>13815126.050000001</v>
+      </c>
+      <c r="T27">
+        <v>2.6869620000000002E-3</v>
+      </c>
+      <c r="U27">
+        <v>3.3457370000000001E-3</v>
+      </c>
+      <c r="V27">
+        <v>312.79288380000003</v>
+      </c>
+      <c r="W27">
+        <v>1025</v>
+      </c>
+      <c r="X27">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y27">
+        <v>1</v>
+      </c>
+      <c r="Z27">
+        <v>2</v>
+      </c>
+      <c r="AA27">
+        <v>2050</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A28">
         <v>103</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D28">
         <v>8.8000000000000007</v>
@@ -2549,18 +3482,51 @@
         <v>4.91</v>
       </c>
       <c r="P28" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q28">
+        <v>0.20340909099999999</v>
+      </c>
+      <c r="R28">
+        <v>1.1965217130000001</v>
+      </c>
+      <c r="S28">
+        <v>14789915.970000001</v>
+      </c>
+      <c r="T28">
+        <v>2.6505700000000001E-3</v>
+      </c>
+      <c r="U28">
+        <v>3.171465E-3</v>
+      </c>
+      <c r="V28">
+        <v>317.42117180000002</v>
+      </c>
+      <c r="W28">
+        <v>1025</v>
+      </c>
+      <c r="X28">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y28">
+        <v>1</v>
+      </c>
+      <c r="Z28">
+        <v>2</v>
+      </c>
+      <c r="AA28">
+        <v>2050</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A29">
         <v>104</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D29">
         <v>10.199999999999999</v>
@@ -2599,18 +3565,51 @@
         <v>4.895480944</v>
       </c>
       <c r="P29" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q29">
+        <v>0.204270022</v>
+      </c>
+      <c r="R29">
+        <v>1.1981474999999999</v>
+      </c>
+      <c r="S29">
+        <v>17142857.140000001</v>
+      </c>
+      <c r="T29">
+        <v>2.573451E-3</v>
+      </c>
+      <c r="U29">
+        <v>3.0833739999999998E-3</v>
+      </c>
+      <c r="V29">
+        <v>357.70053719999999</v>
+      </c>
+      <c r="W29">
+        <v>1025</v>
+      </c>
+      <c r="X29">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y29">
+        <v>1</v>
+      </c>
+      <c r="Z29">
+        <v>2</v>
+      </c>
+      <c r="AA29">
+        <v>2050</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A30">
         <v>105</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D30">
         <v>12.73</v>
@@ -2649,18 +3648,51 @@
         <v>4.7634935509999998</v>
       </c>
       <c r="P30" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q30">
+        <v>0.209929958</v>
+      </c>
+      <c r="R30">
+        <v>1.209041077</v>
+      </c>
+      <c r="S30">
+        <v>21394957.98</v>
+      </c>
+      <c r="T30">
+        <v>2.461899E-3</v>
+      </c>
+      <c r="U30">
+        <v>2.976537E-3</v>
+      </c>
+      <c r="V30">
+        <v>430.95601629999999</v>
+      </c>
+      <c r="W30">
+        <v>1025</v>
+      </c>
+      <c r="X30">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y30">
+        <v>1</v>
+      </c>
+      <c r="Z30">
+        <v>2</v>
+      </c>
+      <c r="AA30">
+        <v>2050</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A31">
         <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D31">
         <v>11.64</v>
@@ -2699,18 +3731,51 @@
         <v>4.6182046579999998</v>
       </c>
       <c r="P31" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q31">
+        <v>0.21653436200000001</v>
+      </c>
+      <c r="R31">
+        <v>1.222209447</v>
+      </c>
+      <c r="S31">
+        <v>19563025.210000001</v>
+      </c>
+      <c r="T31">
+        <v>2.5063709999999999E-3</v>
+      </c>
+      <c r="U31">
+        <v>3.0633100000000001E-3</v>
+      </c>
+      <c r="V31">
+        <v>405.54326140000001</v>
+      </c>
+      <c r="W31">
+        <v>1025</v>
+      </c>
+      <c r="X31">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y31">
+        <v>1</v>
+      </c>
+      <c r="Z31">
+        <v>2</v>
+      </c>
+      <c r="AA31">
+        <v>2050</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A32">
         <v>107</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D32">
         <v>10.55</v>
@@ -2749,18 +3814,51 @@
         <v>5.2121086950000004</v>
       </c>
       <c r="P32" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q32">
+        <v>0.19186092599999999</v>
+      </c>
+      <c r="R32">
+        <v>1.175495819</v>
+      </c>
+      <c r="S32">
+        <v>17731092.440000001</v>
+      </c>
+      <c r="T32">
+        <v>2.5561440000000002E-3</v>
+      </c>
+      <c r="U32">
+        <v>3.0047369999999999E-3</v>
+      </c>
+      <c r="V32">
+        <v>360.53897990000002</v>
+      </c>
+      <c r="W32">
+        <v>1025</v>
+      </c>
+      <c r="X32">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y32">
+        <v>1</v>
+      </c>
+      <c r="Z32">
+        <v>2</v>
+      </c>
+      <c r="AA32">
+        <v>2050</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A33">
         <v>108</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C33" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D33">
         <v>14.76</v>
@@ -2799,18 +3897,51 @@
         <v>4.9055099630000001</v>
       </c>
       <c r="P33" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q33">
+        <v>0.20385240399999999</v>
+      </c>
+      <c r="R33">
+        <v>1.197357845</v>
+      </c>
+      <c r="S33">
+        <v>24806722.690000001</v>
+      </c>
+      <c r="T33">
+        <v>2.390114E-3</v>
+      </c>
+      <c r="U33">
+        <v>2.861822E-3</v>
+      </c>
+      <c r="V33">
+        <v>480.4212612</v>
+      </c>
+      <c r="W33">
+        <v>1025</v>
+      </c>
+      <c r="X33">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y33">
+        <v>1</v>
+      </c>
+      <c r="Z33">
+        <v>2</v>
+      </c>
+      <c r="AA33">
+        <v>2050</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A34">
         <v>109</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D34">
         <v>7.07</v>
@@ -2849,18 +3980,51 @@
         <v>5.0191489100000002</v>
       </c>
       <c r="P34" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q34">
+        <v>0.19923696599999999</v>
+      </c>
+      <c r="R34">
+        <v>1.1887585169999999</v>
+      </c>
+      <c r="S34">
+        <v>11882352.939999999</v>
+      </c>
+      <c r="T34">
+        <v>2.769185E-3</v>
+      </c>
+      <c r="U34">
+        <v>3.2918930000000002E-3</v>
+      </c>
+      <c r="V34">
+        <v>264.70268179999999</v>
+      </c>
+      <c r="W34">
+        <v>1025</v>
+      </c>
+      <c r="X34">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y34">
+        <v>1</v>
+      </c>
+      <c r="Z34">
+        <v>2</v>
+      </c>
+      <c r="AA34">
+        <v>2050</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A35">
         <v>110</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D35">
         <v>9.7799999999999994</v>
@@ -2899,18 +4063,51 @@
         <v>5.2651685959999996</v>
       </c>
       <c r="P35" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q35">
+        <v>0.189927441</v>
+      </c>
+      <c r="R35">
+        <v>1.1721154789999999</v>
+      </c>
+      <c r="S35">
+        <v>16436974.789999999</v>
+      </c>
+      <c r="T35">
+        <v>2.5951839999999999E-3</v>
+      </c>
+      <c r="U35">
+        <v>3.041855E-3</v>
+      </c>
+      <c r="V35">
+        <v>338.35348499999998</v>
+      </c>
+      <c r="W35">
+        <v>1025</v>
+      </c>
+      <c r="X35">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y35">
+        <v>1</v>
+      </c>
+      <c r="Z35">
+        <v>2</v>
+      </c>
+      <c r="AA35">
+        <v>2050</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A36">
         <v>111</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D36">
         <v>12.21</v>
@@ -2949,18 +4146,51 @@
         <v>4.3748130180000002</v>
       </c>
       <c r="P36" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q36">
+        <v>0.22858119800000001</v>
+      </c>
+      <c r="R36">
+        <v>1.247530131</v>
+      </c>
+      <c r="S36">
+        <v>20521008.399999999</v>
+      </c>
+      <c r="T36">
+        <v>2.4825200000000002E-3</v>
+      </c>
+      <c r="U36">
+        <v>3.0970189999999999E-3</v>
+      </c>
+      <c r="V36">
+        <v>430.08346280000001</v>
+      </c>
+      <c r="W36">
+        <v>1025</v>
+      </c>
+      <c r="X36">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y36">
+        <v>1</v>
+      </c>
+      <c r="Z36">
+        <v>2</v>
+      </c>
+      <c r="AA36">
+        <v>2050</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A37">
         <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D37">
         <v>11.69</v>
@@ -2999,18 +4229,51 @@
         <v>4.1293250830000003</v>
       </c>
       <c r="P37" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q37">
+        <v>0.24217032599999999</v>
+      </c>
+      <c r="R37">
+        <v>1.2781779849999999</v>
+      </c>
+      <c r="S37">
+        <v>19647058.82</v>
+      </c>
+      <c r="T37">
+        <v>2.5042229999999999E-3</v>
+      </c>
+      <c r="U37">
+        <v>3.2008430000000001E-3</v>
+      </c>
+      <c r="V37">
+        <v>425.5710833</v>
+      </c>
+      <c r="W37">
+        <v>1025</v>
+      </c>
+      <c r="X37">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y37">
+        <v>1</v>
+      </c>
+      <c r="Z37">
+        <v>2</v>
+      </c>
+      <c r="AA37">
+        <v>2050</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A38">
         <v>113</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="C38" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D38">
         <v>11.97</v>
@@ -3049,18 +4312,51 @@
         <v>4.7244788509999998</v>
       </c>
       <c r="P38" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q38">
+        <v>0.211663557</v>
+      </c>
+      <c r="R38">
+        <v>1.2124496440000001</v>
+      </c>
+      <c r="S38">
+        <v>20117647.059999999</v>
+      </c>
+      <c r="T38">
+        <v>2.492396E-3</v>
+      </c>
+      <c r="U38">
+        <v>3.0219050000000001E-3</v>
+      </c>
+      <c r="V38">
+        <v>411.40370589999998</v>
+      </c>
+      <c r="W38">
+        <v>1025</v>
+      </c>
+      <c r="X38">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y38">
+        <v>1</v>
+      </c>
+      <c r="Z38">
+        <v>2</v>
+      </c>
+      <c r="AA38">
+        <v>2050</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A39">
         <v>114</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="C39" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D39">
         <v>13.13</v>
@@ -3099,18 +4395,51 @@
         <v>5.3941953810000003</v>
       </c>
       <c r="P39" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q39">
+        <v>0.18538446</v>
+      </c>
+      <c r="R39">
+        <v>1.164327793</v>
+      </c>
+      <c r="S39">
+        <v>22067226.890000001</v>
+      </c>
+      <c r="T39">
+        <v>2.4467130000000001E-3</v>
+      </c>
+      <c r="U39">
+        <v>2.848775E-3</v>
+      </c>
+      <c r="V39">
+        <v>425.41834549999999</v>
+      </c>
+      <c r="W39">
+        <v>1025</v>
+      </c>
+      <c r="X39">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y39">
+        <v>1</v>
+      </c>
+      <c r="Z39">
+        <v>2</v>
+      </c>
+      <c r="AA39">
+        <v>2050</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A40">
         <v>115</v>
       </c>
       <c r="B40" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D40">
         <v>10.6</v>
@@ -3149,18 +4478,51 @@
         <v>4.3001587130000001</v>
       </c>
       <c r="P40" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q40">
+        <v>0.23254955599999999</v>
+      </c>
+      <c r="R40">
+        <v>1.2562477409999999</v>
+      </c>
+      <c r="S40">
+        <v>17815126.050000001</v>
+      </c>
+      <c r="T40">
+        <v>2.5537279999999999E-3</v>
+      </c>
+      <c r="U40">
+        <v>3.208116E-3</v>
+      </c>
+      <c r="V40">
+        <v>386.76677130000002</v>
+      </c>
+      <c r="W40">
+        <v>1025</v>
+      </c>
+      <c r="X40">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y40">
+        <v>1</v>
+      </c>
+      <c r="Z40">
+        <v>2</v>
+      </c>
+      <c r="AA40">
+        <v>2050</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A41">
         <v>116</v>
       </c>
       <c r="B41" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="C41" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D41">
         <v>14.74</v>
@@ -3193,21 +4555,54 @@
         <v>1.39</v>
       </c>
       <c r="P41" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>52</v>
+        <v>28</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <v>1</v>
+      </c>
+      <c r="S41">
+        <v>24773109.239999998</v>
+      </c>
+      <c r="T41">
+        <v>2.3907619999999998E-3</v>
+      </c>
+      <c r="U41">
+        <v>2.3907619999999998E-3</v>
+      </c>
+      <c r="V41">
+        <v>400.79948589999998</v>
+      </c>
+      <c r="W41">
+        <v>1025</v>
+      </c>
+      <c r="X41">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y41">
+        <v>1</v>
+      </c>
+      <c r="Z41">
+        <v>2</v>
+      </c>
+      <c r="AA41">
+        <v>2050</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A42">
         <v>124</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D42">
         <v>10.395281069999999</v>
@@ -3246,18 +4641,51 @@
         <v>4.2019872009999997</v>
       </c>
       <c r="P42" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q42">
+        <v>0.237982638</v>
+      </c>
+      <c r="R42">
+        <v>1.268492516</v>
+      </c>
+      <c r="S42">
+        <v>17471060.620000001</v>
+      </c>
+      <c r="T42">
+        <v>2.563708E-3</v>
+      </c>
+      <c r="U42">
+        <v>3.2520449999999998E-3</v>
+      </c>
+      <c r="V42">
+        <v>384.49090169999999</v>
+      </c>
+      <c r="W42">
+        <v>1025</v>
+      </c>
+      <c r="X42">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y42">
+        <v>1</v>
+      </c>
+      <c r="Z42">
+        <v>2</v>
+      </c>
+      <c r="AA42">
+        <v>2050</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A43">
         <v>125</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D43">
         <v>11.98875855</v>
@@ -3296,21 +4724,54 @@
         <v>4.56296284</v>
       </c>
       <c r="P43" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>55</v>
+        <v>30</v>
+      </c>
+      <c r="Q43">
+        <v>0.21915585000000001</v>
+      </c>
+      <c r="R43">
+        <v>1.2275750009999999</v>
+      </c>
+      <c r="S43">
+        <v>20149174.030000001</v>
+      </c>
+      <c r="T43">
+        <v>2.4916159999999999E-3</v>
+      </c>
+      <c r="U43">
+        <v>3.058645E-3</v>
+      </c>
+      <c r="V43">
+        <v>417.05811460000001</v>
+      </c>
+      <c r="W43">
+        <v>1025</v>
+      </c>
+      <c r="X43">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y43">
+        <v>1</v>
+      </c>
+      <c r="Z43">
+        <v>2</v>
+      </c>
+      <c r="AA43">
+        <v>2050</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A44">
         <v>126</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="C44" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D44">
         <v>10.005313230000001</v>
@@ -3349,21 +4810,54 @@
         <v>4.859685721</v>
       </c>
       <c r="P44" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>57</v>
+        <v>28</v>
+      </c>
+      <c r="Q44">
+        <v>0.20577462399999999</v>
+      </c>
+      <c r="R44">
+        <v>1.2010085100000001</v>
+      </c>
+      <c r="S44">
+        <v>16815652.489999998</v>
+      </c>
+      <c r="T44">
+        <v>2.5833890000000002E-3</v>
+      </c>
+      <c r="U44">
+        <v>3.1026719999999999E-3</v>
+      </c>
+      <c r="V44">
+        <v>353.06917700000002</v>
+      </c>
+      <c r="W44">
+        <v>1025</v>
+      </c>
+      <c r="X44">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y44">
+        <v>1</v>
+      </c>
+      <c r="Z44">
+        <v>2</v>
+      </c>
+      <c r="AA44">
+        <v>2050</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A45">
         <v>127</v>
       </c>
       <c r="B45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" t="s">
         <v>58</v>
-      </c>
-      <c r="C45" t="s">
-        <v>33</v>
       </c>
       <c r="D45">
         <v>11.428225319999999</v>
@@ -3402,18 +4896,51 @@
         <v>4.2400303609999996</v>
       </c>
       <c r="P45" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q45">
+        <v>0.235847368</v>
+      </c>
+      <c r="R45">
+        <v>1.2636371820000001</v>
+      </c>
+      <c r="S45">
+        <v>19207101.379999999</v>
+      </c>
+      <c r="T45">
+        <v>2.5155920000000001E-3</v>
+      </c>
+      <c r="U45">
+        <v>3.1787949999999999E-3</v>
+      </c>
+      <c r="V45">
+        <v>413.17553759999998</v>
+      </c>
+      <c r="W45">
+        <v>1025</v>
+      </c>
+      <c r="X45">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y45">
+        <v>1</v>
+      </c>
+      <c r="Z45">
+        <v>2</v>
+      </c>
+      <c r="AA45">
+        <v>2050</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A46">
         <v>128</v>
       </c>
       <c r="B46" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="C46" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D46">
         <v>10.661631079999999</v>
@@ -3452,18 +4979,51 @@
         <v>4.5937232459999997</v>
       </c>
       <c r="P46" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q46">
+        <v>0.21768834300000001</v>
+      </c>
+      <c r="R46">
+        <v>1.22456158</v>
+      </c>
+      <c r="S46">
+        <v>17918707.699999999</v>
+      </c>
+      <c r="T46">
+        <v>2.550769E-3</v>
+      </c>
+      <c r="U46">
+        <v>3.1235740000000001E-3</v>
+      </c>
+      <c r="V46">
+        <v>378.76402180000002</v>
+      </c>
+      <c r="W46">
+        <v>1025</v>
+      </c>
+      <c r="X46">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y46">
+        <v>1</v>
+      </c>
+      <c r="Z46">
+        <v>2</v>
+      </c>
+      <c r="AA46">
+        <v>2050</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A47">
         <v>129</v>
       </c>
       <c r="B47" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="C47" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D47">
         <v>9.4238525580000001</v>
@@ -3502,18 +5062,51 @@
         <v>4.7222207980000004</v>
       </c>
       <c r="P47" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q47">
+        <v>0.21176476999999999</v>
+      </c>
+      <c r="R47">
+        <v>1.2126496959999999</v>
+      </c>
+      <c r="S47">
+        <v>15838407.66</v>
+      </c>
+      <c r="T47">
+        <v>2.6145090000000001E-3</v>
+      </c>
+      <c r="U47">
+        <v>3.1704839999999999E-3</v>
+      </c>
+      <c r="V47">
+        <v>339.81873389999998</v>
+      </c>
+      <c r="W47">
+        <v>1025</v>
+      </c>
+      <c r="X47">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y47">
+        <v>1</v>
+      </c>
+      <c r="Z47">
+        <v>2</v>
+      </c>
+      <c r="AA47">
+        <v>2050</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A48">
         <v>130</v>
       </c>
       <c r="B48" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="C48" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D48">
         <v>11.379433130000001</v>
@@ -3552,18 +5145,51 @@
         <v>4.8470943379999998</v>
       </c>
       <c r="P48" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q48">
+        <v>0.20630916799999999</v>
+      </c>
+      <c r="R48">
+        <v>1.2020310059999999</v>
+      </c>
+      <c r="S48">
+        <v>19125097.699999999</v>
+      </c>
+      <c r="T48">
+        <v>2.5177450000000001E-3</v>
+      </c>
+      <c r="U48">
+        <v>3.026408E-3</v>
+      </c>
+      <c r="V48">
+        <v>391.68896960000001</v>
+      </c>
+      <c r="W48">
+        <v>1025</v>
+      </c>
+      <c r="X48">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y48">
+        <v>1</v>
+      </c>
+      <c r="Z48">
+        <v>2</v>
+      </c>
+      <c r="AA48">
+        <v>2050</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A49">
         <v>131</v>
       </c>
       <c r="B49" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D49">
         <v>11.359311440000001</v>
@@ -3602,21 +5228,54 @@
         <v>4.8013278650000002</v>
       </c>
       <c r="P49" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>102</v>
+        <v>28</v>
+      </c>
+      <c r="Q49">
+        <v>0.208275716</v>
+      </c>
+      <c r="R49">
+        <v>1.2058201319999999</v>
+      </c>
+      <c r="S49">
+        <v>19091279.73</v>
+      </c>
+      <c r="T49">
+        <v>2.5186359999999999E-3</v>
+      </c>
+      <c r="U49">
+        <v>3.0370229999999998E-3</v>
+      </c>
+      <c r="V49">
+        <v>392.36775080000001</v>
+      </c>
+      <c r="W49">
+        <v>1025</v>
+      </c>
+      <c r="X49">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y49">
+        <v>1</v>
+      </c>
+      <c r="Z49">
+        <v>2</v>
+      </c>
+      <c r="AA49">
+        <v>2050</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A50" s="1">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A50">
         <v>144</v>
       </c>
       <c r="B50" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="C50" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D50">
         <v>12.93</v>
@@ -3655,18 +5314,51 @@
         <v>4.824626866</v>
       </c>
       <c r="P50" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q50">
+        <v>0.207269915</v>
+      </c>
+      <c r="R50">
+        <v>1.203876763</v>
+      </c>
+      <c r="S50">
+        <v>21731092.440000001</v>
+      </c>
+      <c r="T50">
+        <v>2.4542349999999999E-3</v>
+      </c>
+      <c r="U50">
+        <v>2.9545970000000002E-3</v>
+      </c>
+      <c r="V50">
+        <v>434.50024020000001</v>
+      </c>
+      <c r="W50">
+        <v>1025</v>
+      </c>
+      <c r="X50">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y50">
+        <v>1</v>
+      </c>
+      <c r="Z50">
+        <v>2</v>
+      </c>
+      <c r="AA50">
+        <v>2050</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A51">
         <v>145</v>
       </c>
       <c r="B51" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="C51" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D51">
         <v>12.38</v>
@@ -3705,18 +5397,51 @@
         <v>5.4298245610000002</v>
       </c>
       <c r="P51" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q51">
+        <v>0.18416801299999999</v>
+      </c>
+      <c r="R51">
+        <v>1.1622790940000001</v>
+      </c>
+      <c r="S51">
+        <v>20806722.690000001</v>
+      </c>
+      <c r="T51">
+        <v>2.4756639999999998E-3</v>
+      </c>
+      <c r="U51">
+        <v>2.8774130000000001E-3</v>
+      </c>
+      <c r="V51">
+        <v>405.15024979999998</v>
+      </c>
+      <c r="W51">
+        <v>1025</v>
+      </c>
+      <c r="X51">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y51">
+        <v>1</v>
+      </c>
+      <c r="Z51">
+        <v>2</v>
+      </c>
+      <c r="AA51">
+        <v>2050</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A52" s="1">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A52">
         <v>146</v>
       </c>
       <c r="B52" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="C52" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D52">
         <v>7.82</v>
@@ -3755,18 +5480,51 @@
         <v>5.75</v>
       </c>
       <c r="P52" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q52">
+        <v>0.17391304299999999</v>
+      </c>
+      <c r="R52">
+        <v>1.145611038</v>
+      </c>
+      <c r="S52">
+        <v>13142857.140000001</v>
+      </c>
+      <c r="T52">
+        <v>2.7139040000000001E-3</v>
+      </c>
+      <c r="U52">
+        <v>3.1090789999999998E-3</v>
+      </c>
+      <c r="V52">
+        <v>276.52331900000001</v>
+      </c>
+      <c r="W52">
+        <v>1025</v>
+      </c>
+      <c r="X52">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y52">
+        <v>1</v>
+      </c>
+      <c r="Z52">
+        <v>2</v>
+      </c>
+      <c r="AA52">
+        <v>2050</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A53" s="1">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A53">
         <v>147</v>
       </c>
       <c r="B53" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="C53" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D53">
         <v>13.1</v>
@@ -3805,18 +5563,51 @@
         <v>5.019157088</v>
       </c>
       <c r="P53" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q53">
+        <v>0.19923664099999999</v>
+      </c>
+      <c r="R53">
+        <v>1.18875792</v>
+      </c>
+      <c r="S53">
+        <v>22016806.719999999</v>
+      </c>
+      <c r="T53">
+        <v>2.447832E-3</v>
+      </c>
+      <c r="U53">
+        <v>2.9098800000000001E-3</v>
+      </c>
+      <c r="V53">
+        <v>433.55043760000001</v>
+      </c>
+      <c r="W53">
+        <v>1025</v>
+      </c>
+      <c r="X53">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y53">
+        <v>1</v>
+      </c>
+      <c r="Z53">
+        <v>2</v>
+      </c>
+      <c r="AA53">
+        <v>2050</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A54">
         <v>148</v>
       </c>
       <c r="B54" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="C54" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D54">
         <v>9.99</v>
@@ -3855,18 +5646,51 @@
         <v>4.6465116279999998</v>
       </c>
       <c r="P54" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q54">
+        <v>0.21521521499999999</v>
+      </c>
+      <c r="R54">
+        <v>1.2195394340000001</v>
+      </c>
+      <c r="S54">
+        <v>16789915.969999999</v>
+      </c>
+      <c r="T54">
+        <v>2.5841800000000002E-3</v>
+      </c>
+      <c r="U54">
+        <v>3.1515100000000002E-3</v>
+      </c>
+      <c r="V54">
+        <v>358.07780880000001</v>
+      </c>
+      <c r="W54">
+        <v>1025</v>
+      </c>
+      <c r="X54">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y54">
+        <v>1</v>
+      </c>
+      <c r="Z54">
+        <v>2</v>
+      </c>
+      <c r="AA54">
+        <v>2050</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A55" s="1">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A55">
         <v>156</v>
       </c>
       <c r="B55" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="C55" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D55">
         <v>4.54</v>
@@ -3905,18 +5729,51 @@
         <v>4.9397953729999999</v>
       </c>
       <c r="P55" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q55">
+        <v>0.202437535</v>
+      </c>
+      <c r="R55">
+        <v>1.194696845</v>
+      </c>
+      <c r="S55">
+        <v>7630252.1009999998</v>
+      </c>
+      <c r="T55">
+        <v>3.025692E-3</v>
+      </c>
+      <c r="U55">
+        <v>3.6147850000000001E-3</v>
+      </c>
+      <c r="V55">
+        <v>117.74980429999999</v>
+      </c>
+      <c r="W55">
+        <v>1025</v>
+      </c>
+      <c r="X55">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y55">
+        <v>1</v>
+      </c>
+      <c r="Z55">
+        <v>2</v>
+      </c>
+      <c r="AA55">
+        <v>2050</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A56" s="1">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A56">
         <v>157</v>
       </c>
       <c r="B56" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="C56" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D56">
         <v>5.76</v>
@@ -3955,18 +5812,51 @@
         <v>5.459923034</v>
       </c>
       <c r="P56" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q56">
+        <v>0.183152765</v>
+      </c>
+      <c r="R56">
+        <v>1.160580983</v>
+      </c>
+      <c r="S56">
+        <v>9680672.2689999994</v>
+      </c>
+      <c r="T56">
+        <v>2.885037E-3</v>
+      </c>
+      <c r="U56">
+        <v>3.3483190000000002E-3</v>
+      </c>
+      <c r="V56">
+        <v>138.37933269999999</v>
+      </c>
+      <c r="W56">
+        <v>1025</v>
+      </c>
+      <c r="X56">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y56">
+        <v>1</v>
+      </c>
+      <c r="Z56">
+        <v>2</v>
+      </c>
+      <c r="AA56">
+        <v>2050</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A57" s="1">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A57">
         <v>158</v>
       </c>
       <c r="B57" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="C57" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D57">
         <v>7.96</v>
@@ -4005,18 +5895,51 @@
         <v>6.5433385609999997</v>
       </c>
       <c r="P57" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q57">
+        <v>0.15282718300000001</v>
+      </c>
+      <c r="R57">
+        <v>1.114603545</v>
+      </c>
+      <c r="S57">
+        <v>13378151.26</v>
+      </c>
+      <c r="T57">
+        <v>2.7042899999999998E-3</v>
+      </c>
+      <c r="U57">
+        <v>3.0142110000000001E-3</v>
+      </c>
+      <c r="V57">
+        <v>172.15065100000001</v>
+      </c>
+      <c r="W57">
+        <v>1025</v>
+      </c>
+      <c r="X57">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y57">
+        <v>1</v>
+      </c>
+      <c r="Z57">
+        <v>2</v>
+      </c>
+      <c r="AA57">
+        <v>2050</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A58" s="1">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A58">
         <v>159</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D58">
         <v>8.7899999999999991</v>
@@ -4055,18 +5978,51 @@
         <v>6.3829842990000003</v>
       </c>
       <c r="P58" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q58">
+        <v>0.15666653</v>
+      </c>
+      <c r="R58">
+        <v>1.1199325609999999</v>
+      </c>
+      <c r="S58">
+        <v>14773109.24</v>
+      </c>
+      <c r="T58">
+        <v>2.6511730000000002E-3</v>
+      </c>
+      <c r="U58">
+        <v>2.9691349999999999E-3</v>
+      </c>
+      <c r="V58">
+        <v>187.25816649999999</v>
+      </c>
+      <c r="W58">
+        <v>1025</v>
+      </c>
+      <c r="X58">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y58">
+        <v>1</v>
+      </c>
+      <c r="Z58">
+        <v>2</v>
+      </c>
+      <c r="AA58">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>160</v>
+      </c>
+      <c r="B59" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A59" s="1">
-        <v>160</v>
-      </c>
-      <c r="B59" t="s">
-        <v>72</v>
-      </c>
       <c r="C59" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D59">
         <v>6.53</v>
@@ -4105,18 +6061,51 @@
         <v>6.4642058330000003</v>
       </c>
       <c r="P59" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q59">
+        <v>0.15469804400000001</v>
+      </c>
+      <c r="R59">
+        <v>1.117183069</v>
+      </c>
+      <c r="S59">
+        <v>10974789.92</v>
+      </c>
+      <c r="T59">
+        <v>2.8135410000000001E-3</v>
+      </c>
+      <c r="U59">
+        <v>3.1432399999999998E-3</v>
+      </c>
+      <c r="V59">
+        <v>147.26945689999999</v>
+      </c>
+      <c r="W59">
+        <v>1025</v>
+      </c>
+      <c r="X59">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y59">
+        <v>1</v>
+      </c>
+      <c r="Z59">
+        <v>2</v>
+      </c>
+      <c r="AA59">
+        <v>2050</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A60" s="1">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A60">
         <v>161</v>
       </c>
       <c r="B60" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="C60" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D60">
         <v>6.56</v>
@@ -4155,18 +6144,51 @@
         <v>5.8028054850000004</v>
       </c>
       <c r="P60" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q60">
+        <v>0.172330436</v>
+      </c>
+      <c r="R60">
+        <v>1.143133347</v>
+      </c>
+      <c r="S60">
+        <v>11025210.08</v>
+      </c>
+      <c r="T60">
+        <v>2.8109630000000001E-3</v>
+      </c>
+      <c r="U60">
+        <v>3.2133050000000001E-3</v>
+      </c>
+      <c r="V60">
+        <v>151.24386269999999</v>
+      </c>
+      <c r="W60">
+        <v>1025</v>
+      </c>
+      <c r="X60">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y60">
+        <v>1</v>
+      </c>
+      <c r="Z60">
+        <v>2</v>
+      </c>
+      <c r="AA60">
+        <v>2050</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A61" s="1">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A61">
         <v>162</v>
       </c>
       <c r="B61" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="C61" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D61">
         <v>5.97</v>
@@ -4205,18 +6227,51 @@
         <v>5.4554112569999997</v>
       </c>
       <c r="P61" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q61">
+        <v>0.18330423700000001</v>
+      </c>
+      <c r="R61">
+        <v>1.1608336610000001</v>
+      </c>
+      <c r="S61">
+        <v>10033613.449999999</v>
+      </c>
+      <c r="T61">
+        <v>2.8644489999999998E-3</v>
+      </c>
+      <c r="U61">
+        <v>3.325148E-3</v>
+      </c>
+      <c r="V61">
+        <v>142.43189520000001</v>
+      </c>
+      <c r="W61">
+        <v>1025</v>
+      </c>
+      <c r="X61">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y61">
+        <v>1</v>
+      </c>
+      <c r="Z61">
+        <v>2</v>
+      </c>
+      <c r="AA61">
+        <v>2050</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A62" s="1">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A62">
         <v>163</v>
       </c>
       <c r="B62" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="C62" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D62">
         <v>8.4700000000000006</v>
@@ -4255,18 +6310,51 @@
         <v>5.9409134479999999</v>
       </c>
       <c r="P62" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q62">
+        <v>0.16832428399999999</v>
+      </c>
+      <c r="R62">
+        <v>1.1369724699999999</v>
+      </c>
+      <c r="S62">
+        <v>14235294.119999999</v>
+      </c>
+      <c r="T62">
+        <v>2.6709099999999999E-3</v>
+      </c>
+      <c r="U62">
+        <v>3.0367509999999999E-3</v>
+      </c>
+      <c r="V62">
+        <v>184.5501797</v>
+      </c>
+      <c r="W62">
+        <v>1025</v>
+      </c>
+      <c r="X62">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y62">
+        <v>1</v>
+      </c>
+      <c r="Z62">
+        <v>2</v>
+      </c>
+      <c r="AA62">
+        <v>2050</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A63" s="1">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A63">
         <v>164</v>
       </c>
       <c r="B63" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D63">
         <v>7.06</v>
@@ -4305,18 +6393,51 @@
         <v>5.7314734639999996</v>
       </c>
       <c r="P63" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q63">
+        <v>0.17447520399999999</v>
+      </c>
+      <c r="R63">
+        <v>1.146497165</v>
+      </c>
+      <c r="S63">
+        <v>11865546.220000001</v>
+      </c>
+      <c r="T63">
+        <v>2.7699690000000002E-3</v>
+      </c>
+      <c r="U63">
+        <v>3.1757619999999999E-3</v>
+      </c>
+      <c r="V63">
+        <v>160.8698071</v>
+      </c>
+      <c r="W63">
+        <v>1025</v>
+      </c>
+      <c r="X63">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y63">
+        <v>1</v>
+      </c>
+      <c r="Z63">
+        <v>2</v>
+      </c>
+      <c r="AA63">
+        <v>2050</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A64" s="1">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A64">
         <v>165</v>
       </c>
       <c r="B64" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="C64" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D64">
         <v>8.6199999999999992</v>
@@ -4355,18 +6476,51 @@
         <v>5.5060444520000003</v>
       </c>
       <c r="P64" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q64">
+        <v>0.181618585</v>
+      </c>
+      <c r="R64">
+        <v>1.158035076</v>
+      </c>
+      <c r="S64">
+        <v>14487394.960000001</v>
+      </c>
+      <c r="T64">
+        <v>2.661549E-3</v>
+      </c>
+      <c r="U64">
+        <v>3.0821669999999998E-3</v>
+      </c>
+      <c r="V64">
+        <v>190.62739869999999</v>
+      </c>
+      <c r="W64">
+        <v>1025</v>
+      </c>
+      <c r="X64">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y64">
+        <v>1</v>
+      </c>
+      <c r="Z64">
+        <v>2</v>
+      </c>
+      <c r="AA64">
+        <v>2050</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A65" s="1">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A65">
         <v>166</v>
       </c>
       <c r="B65" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D65">
         <v>8.09</v>
@@ -4402,21 +6556,54 @@
         <v>1.505379611</v>
       </c>
       <c r="O65">
-        <v>5.3740597659788554</v>
+        <v>5.3740597660000002</v>
       </c>
       <c r="P65" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q65">
+        <v>0.18607906199999999</v>
+      </c>
+      <c r="R65">
+        <v>1.1655045150000001</v>
+      </c>
+      <c r="S65">
+        <v>13596638.66</v>
+      </c>
+      <c r="T65">
+        <v>2.6955429999999999E-3</v>
+      </c>
+      <c r="U65">
+        <v>3.1416669999999999E-3</v>
+      </c>
+      <c r="V65">
+        <v>182.3604153</v>
+      </c>
+      <c r="W65">
+        <v>1025</v>
+      </c>
+      <c r="X65">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y65">
+        <v>1</v>
+      </c>
+      <c r="Z65">
+        <v>2</v>
+      </c>
+      <c r="AA65">
+        <v>2050</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A66" s="1">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A66">
         <v>167</v>
       </c>
       <c r="B66" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="C66" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D66">
         <v>7.16</v>
@@ -4452,21 +6639,54 @@
         <v>0.96832205100000002</v>
       </c>
       <c r="O66">
-        <v>7.394234173027213</v>
+        <v>7.3942341730000001</v>
       </c>
       <c r="P66" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q66">
+        <v>0.13524051000000001</v>
+      </c>
+      <c r="R66">
+        <v>1.091917008</v>
+      </c>
+      <c r="S66">
+        <v>12033613.449999999</v>
+      </c>
+      <c r="T66">
+        <v>2.7621880000000001E-3</v>
+      </c>
+      <c r="U66">
+        <v>3.01608E-3</v>
+      </c>
+      <c r="V66">
+        <v>154.9450989</v>
+      </c>
+      <c r="W66">
+        <v>1025</v>
+      </c>
+      <c r="X66">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y66">
+        <v>1</v>
+      </c>
+      <c r="Z66">
+        <v>2</v>
+      </c>
+      <c r="AA66">
+        <v>2050</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A67" s="1">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A67">
         <v>168</v>
       </c>
       <c r="B67" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="C67" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="D67">
         <v>9.9700000000000006</v>
@@ -4499,21 +6719,54 @@
         <v>1.2569999999999999</v>
       </c>
       <c r="O67">
-        <v>7.9315831344470977</v>
+        <v>7.9315831340000003</v>
       </c>
       <c r="P67" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q67">
+        <v>0.12607823500000001</v>
+      </c>
+      <c r="R67">
+        <v>1.08117957</v>
+      </c>
+      <c r="S67">
+        <v>16756302.52</v>
+      </c>
+      <c r="T67">
+        <v>2.585216E-3</v>
+      </c>
+      <c r="U67">
+        <v>2.7950829999999999E-3</v>
+      </c>
+      <c r="V67">
+        <v>200.1192351</v>
+      </c>
+      <c r="W67">
+        <v>1025</v>
+      </c>
+      <c r="X67">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y67">
+        <v>1</v>
+      </c>
+      <c r="Z67">
+        <v>2</v>
+      </c>
+      <c r="AA67">
+        <v>2050</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A68" s="1">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A68">
         <v>169</v>
       </c>
       <c r="B68" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="C68" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="D68">
         <v>14.1</v>
@@ -4546,21 +6799,54 @@
         <v>1.994</v>
       </c>
       <c r="O68">
-        <v>7.0712136409227684</v>
+        <v>7.0712136409999999</v>
       </c>
       <c r="P68" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q68">
+        <v>0.14141844000000001</v>
+      </c>
+      <c r="R68">
+        <v>1.0995697360000001</v>
+      </c>
+      <c r="S68">
+        <v>23697478.989999998</v>
+      </c>
+      <c r="T68">
+        <v>2.4120819999999999E-3</v>
+      </c>
+      <c r="U68">
+        <v>2.6522519999999999E-3</v>
+      </c>
+      <c r="V68">
+        <v>368.17551320000001</v>
+      </c>
+      <c r="W68">
+        <v>1025</v>
+      </c>
+      <c r="X68">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y68">
+        <v>1</v>
+      </c>
+      <c r="Z68">
+        <v>2</v>
+      </c>
+      <c r="AA68">
+        <v>2050</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A69" s="1">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A69">
         <v>170</v>
       </c>
       <c r="B69" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="C69" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="D69">
         <v>16.62</v>
@@ -4593,21 +6879,54 @@
         <v>1.9330000000000001</v>
       </c>
       <c r="O69">
-        <v>8.5980341438179</v>
+        <v>8.5980341439999997</v>
       </c>
       <c r="P69" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q69">
+        <v>0.11630565599999999</v>
+      </c>
+      <c r="R69">
+        <v>1.0705095200000001</v>
+      </c>
+      <c r="S69">
+        <v>27932773.109999999</v>
+      </c>
+      <c r="T69">
+        <v>2.3340470000000001E-3</v>
+      </c>
+      <c r="U69">
+        <v>2.49862E-3</v>
+      </c>
+      <c r="V69">
+        <v>474.8521854</v>
+      </c>
+      <c r="W69">
+        <v>1025</v>
+      </c>
+      <c r="X69">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y69">
+        <v>1</v>
+      </c>
+      <c r="Z69">
+        <v>2</v>
+      </c>
+      <c r="AA69">
+        <v>2050</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A70" s="1">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A70">
         <v>171</v>
       </c>
       <c r="B70" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="C70" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="D70">
         <v>15.73</v>
@@ -4640,10 +6959,43 @@
         <v>2.0219999999999998</v>
       </c>
       <c r="O70">
-        <v>7.7794263105835819</v>
+        <v>7.7794263109999999</v>
       </c>
       <c r="P70" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="Q70">
+        <v>0.12854418300000001</v>
+      </c>
+      <c r="R70">
+        <v>1.0839986269999999</v>
+      </c>
+      <c r="S70">
+        <v>26436974.789999999</v>
+      </c>
+      <c r="T70">
+        <v>2.3598809999999999E-3</v>
+      </c>
+      <c r="U70">
+        <v>2.5581079999999999E-3</v>
+      </c>
+      <c r="V70">
+        <v>437.63952819999997</v>
+      </c>
+      <c r="W70">
+        <v>1025</v>
+      </c>
+      <c r="X70">
+        <v>1.19E-6</v>
+      </c>
+      <c r="Y70">
+        <v>1</v>
+      </c>
+      <c r="Z70">
+        <v>2</v>
+      </c>
+      <c r="AA70">
+        <v>2050</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update with some Extra figures
</commit_message>
<xml_diff>
--- a/Finalized Data Sheet For Hayden.xlsx
+++ b/Finalized Data Sheet For Hayden.xlsx
@@ -24,9 +24,6 @@
     <t>IDNum</t>
   </si>
   <si>
-    <t>Whale</t>
-  </si>
-  <si>
     <t>Species</t>
   </si>
   <si>
@@ -361,6 +358,9 @@
   </si>
   <si>
     <t>Reynolds Number Model</t>
+  </si>
+  <si>
+    <t>DeployID</t>
   </si>
 </sst>
 </file>
@@ -1169,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1205,85 +1205,85 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>112</v>
+      </c>
+      <c r="T1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
-        <v>113</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
+        <v>111</v>
+      </c>
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
-        <v>112</v>
-      </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
@@ -1291,10 +1291,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
       </c>
       <c r="D2">
         <v>8.0394576559999997</v>
@@ -1333,7 +1333,7 @@
         <v>5.6442808539999998</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q2">
         <v>0.17717048899999999</v>
@@ -1374,10 +1374,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3">
         <v>8.6209207879999994</v>
@@ -1416,7 +1416,7 @@
         <v>5.9701104779999996</v>
       </c>
       <c r="P3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q3">
         <v>0.16750108799999999</v>
@@ -1452,7 +1452,7 @@
         <v>2050</v>
       </c>
       <c r="AB3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
@@ -1460,10 +1460,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
         <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
       </c>
       <c r="D4">
         <v>18.47</v>
@@ -1496,7 +1496,7 @@
         <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -1532,7 +1532,7 @@
         <v>2050</v>
       </c>
       <c r="AB4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
@@ -1540,10 +1540,10 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5">
         <v>19.329999999999998</v>
@@ -1582,7 +1582,7 @@
         <v>10.173684209999999</v>
       </c>
       <c r="P5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q5">
         <v>9.8292808999999995E-2</v>
@@ -1623,10 +1623,10 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
         <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
       </c>
       <c r="D6">
         <v>22.59</v>
@@ -1659,7 +1659,7 @@
         <v>1.33</v>
       </c>
       <c r="P6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -1695,7 +1695,7 @@
         <v>2050</v>
       </c>
       <c r="AB6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
@@ -1703,10 +1703,10 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7">
         <v>22.21</v>
@@ -1745,7 +1745,7 @@
         <v>8.1955719560000002</v>
       </c>
       <c r="P7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q7">
         <v>0.122017109</v>
@@ -1786,10 +1786,10 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8">
         <v>22.53</v>
@@ -1828,7 +1828,7 @@
         <v>7.8684503379999997</v>
       </c>
       <c r="P8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q8">
         <v>0.12708982799999999</v>
@@ -1869,10 +1869,10 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9">
         <v>22.75</v>
@@ -1911,7 +1911,7 @@
         <v>7.1745283960000004</v>
       </c>
       <c r="P9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q9">
         <v>0.13938198399999999</v>
@@ -1952,10 +1952,10 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10">
         <v>20.7</v>
@@ -1988,7 +1988,7 @@
         <v>1.04</v>
       </c>
       <c r="P10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -2029,10 +2029,10 @@
         <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11">
         <v>22.55</v>
@@ -2071,7 +2071,7 @@
         <v>8.4591594069999996</v>
       </c>
       <c r="P11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q11">
         <v>0.118215056</v>
@@ -2112,10 +2112,10 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12">
         <v>21.09</v>
@@ -2154,7 +2154,7 @@
         <v>8.2564975080000007</v>
       </c>
       <c r="P12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q12">
         <v>0.121116732</v>
@@ -2195,10 +2195,10 @@
         <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13">
         <v>21.98</v>
@@ -2237,7 +2237,7 @@
         <v>8.0051470079999998</v>
       </c>
       <c r="P13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q13">
         <v>0.12491963</v>
@@ -2278,10 +2278,10 @@
         <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14">
         <v>22.51</v>
@@ -2320,7 +2320,7 @@
         <v>7.2612903229999999</v>
       </c>
       <c r="P14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q14">
         <v>0.13771657000000001</v>
@@ -2361,10 +2361,10 @@
         <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15">
         <v>24.12</v>
@@ -2403,7 +2403,7 @@
         <v>8.3089639940000009</v>
       </c>
       <c r="P15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q15">
         <v>0.120351948</v>
@@ -2444,10 +2444,10 @@
         <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16">
         <v>21.77</v>
@@ -2486,7 +2486,7 @@
         <v>8.1255744110000006</v>
       </c>
       <c r="P16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q16">
         <v>0.123068223</v>
@@ -2527,10 +2527,10 @@
         <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17">
         <v>22.93</v>
@@ -2569,7 +2569,7 @@
         <v>7.8692040710000004</v>
       </c>
       <c r="P17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q17">
         <v>0.12707765500000001</v>
@@ -2610,10 +2610,10 @@
         <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18">
         <v>23.59</v>
@@ -2652,7 +2652,7 @@
         <v>6.8575581400000001</v>
       </c>
       <c r="P18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q18">
         <v>0.14582450199999999</v>
@@ -2693,10 +2693,10 @@
         <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19">
         <v>19.27</v>
@@ -2735,7 +2735,7 @@
         <v>7.9958506219999999</v>
       </c>
       <c r="P19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q19">
         <v>0.125064868</v>
@@ -2776,10 +2776,10 @@
         <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20">
         <v>21.98</v>
@@ -2818,7 +2818,7 @@
         <v>8.1107011070000006</v>
       </c>
       <c r="P20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q20">
         <v>0.123293904</v>
@@ -2859,10 +2859,10 @@
         <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21">
         <v>25.18</v>
@@ -2901,7 +2901,7 @@
         <v>8.7430555559999998</v>
       </c>
       <c r="P21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q21">
         <v>0.114376489</v>
@@ -2942,10 +2942,10 @@
         <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22">
         <v>22.83</v>
@@ -2984,7 +2984,7 @@
         <v>8.1827956989999997</v>
       </c>
       <c r="P22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q22">
         <v>0.122207622</v>
@@ -3020,7 +3020,7 @@
         <v>2050</v>
       </c>
       <c r="AB22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.3">
@@ -3028,10 +3028,10 @@
         <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23">
         <v>24.49</v>
@@ -3070,7 +3070,7 @@
         <v>8.7153024909999992</v>
       </c>
       <c r="P23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q23">
         <v>0.11474071</v>
@@ -3111,10 +3111,10 @@
         <v>98</v>
       </c>
       <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
         <v>57</v>
-      </c>
-      <c r="C24" t="s">
-        <v>58</v>
       </c>
       <c r="D24">
         <v>10.1</v>
@@ -3147,7 +3147,7 @@
         <v>0.94</v>
       </c>
       <c r="P24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q24">
         <v>0</v>
@@ -3183,7 +3183,7 @@
         <v>2050</v>
       </c>
       <c r="AB24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.3">
@@ -3191,10 +3191,10 @@
         <v>99</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D25">
         <v>10.44</v>
@@ -3233,7 +3233,7 @@
         <v>5.3731959099999997</v>
       </c>
       <c r="P25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q25">
         <v>0.18610897800000001</v>
@@ -3274,10 +3274,10 @@
         <v>100</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D26">
         <v>12.17</v>
@@ -3316,7 +3316,7 @@
         <v>5.5748651970000003</v>
       </c>
       <c r="P26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q26">
         <v>0.179376535</v>
@@ -3357,10 +3357,10 @@
         <v>101</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D27">
         <v>8.2200000000000006</v>
@@ -3399,7 +3399,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="P27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q27">
         <v>0.22749391699999999</v>
@@ -3440,10 +3440,10 @@
         <v>103</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D28">
         <v>8.8000000000000007</v>
@@ -3482,7 +3482,7 @@
         <v>4.91</v>
       </c>
       <c r="P28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q28">
         <v>0.20340909099999999</v>
@@ -3523,10 +3523,10 @@
         <v>104</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29">
         <v>10.199999999999999</v>
@@ -3565,7 +3565,7 @@
         <v>4.895480944</v>
       </c>
       <c r="P29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q29">
         <v>0.204270022</v>
@@ -3606,10 +3606,10 @@
         <v>105</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D30">
         <v>12.73</v>
@@ -3648,7 +3648,7 @@
         <v>4.7634935509999998</v>
       </c>
       <c r="P30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q30">
         <v>0.209929958</v>
@@ -3689,10 +3689,10 @@
         <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D31">
         <v>11.64</v>
@@ -3731,7 +3731,7 @@
         <v>4.6182046579999998</v>
       </c>
       <c r="P31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q31">
         <v>0.21653436200000001</v>
@@ -3772,10 +3772,10 @@
         <v>107</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D32">
         <v>10.55</v>
@@ -3814,7 +3814,7 @@
         <v>5.2121086950000004</v>
       </c>
       <c r="P32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q32">
         <v>0.19186092599999999</v>
@@ -3855,10 +3855,10 @@
         <v>108</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D33">
         <v>14.76</v>
@@ -3897,7 +3897,7 @@
         <v>4.9055099630000001</v>
       </c>
       <c r="P33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q33">
         <v>0.20385240399999999</v>
@@ -3938,10 +3938,10 @@
         <v>109</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D34">
         <v>7.07</v>
@@ -3980,7 +3980,7 @@
         <v>5.0191489100000002</v>
       </c>
       <c r="P34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q34">
         <v>0.19923696599999999</v>
@@ -4021,10 +4021,10 @@
         <v>110</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D35">
         <v>9.7799999999999994</v>
@@ -4063,7 +4063,7 @@
         <v>5.2651685959999996</v>
       </c>
       <c r="P35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q35">
         <v>0.189927441</v>
@@ -4104,10 +4104,10 @@
         <v>111</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D36">
         <v>12.21</v>
@@ -4146,7 +4146,7 @@
         <v>4.3748130180000002</v>
       </c>
       <c r="P36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q36">
         <v>0.22858119800000001</v>
@@ -4187,10 +4187,10 @@
         <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D37">
         <v>11.69</v>
@@ -4229,7 +4229,7 @@
         <v>4.1293250830000003</v>
       </c>
       <c r="P37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q37">
         <v>0.24217032599999999</v>
@@ -4270,10 +4270,10 @@
         <v>113</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D38">
         <v>11.97</v>
@@ -4312,7 +4312,7 @@
         <v>4.7244788509999998</v>
       </c>
       <c r="P38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q38">
         <v>0.211663557</v>
@@ -4353,10 +4353,10 @@
         <v>114</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D39">
         <v>13.13</v>
@@ -4395,7 +4395,7 @@
         <v>5.3941953810000003</v>
       </c>
       <c r="P39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q39">
         <v>0.18538446</v>
@@ -4436,10 +4436,10 @@
         <v>115</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D40">
         <v>10.6</v>
@@ -4478,7 +4478,7 @@
         <v>4.3001587130000001</v>
       </c>
       <c r="P40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q40">
         <v>0.23254955599999999</v>
@@ -4519,10 +4519,10 @@
         <v>116</v>
       </c>
       <c r="B41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D41">
         <v>14.74</v>
@@ -4555,7 +4555,7 @@
         <v>1.39</v>
       </c>
       <c r="P41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q41">
         <v>0</v>
@@ -4591,7 +4591,7 @@
         <v>2050</v>
       </c>
       <c r="AB41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
@@ -4599,10 +4599,10 @@
         <v>124</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D42">
         <v>10.395281069999999</v>
@@ -4641,7 +4641,7 @@
         <v>4.2019872009999997</v>
       </c>
       <c r="P42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q42">
         <v>0.237982638</v>
@@ -4682,10 +4682,10 @@
         <v>125</v>
       </c>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D43">
         <v>11.98875855</v>
@@ -4724,7 +4724,7 @@
         <v>4.56296284</v>
       </c>
       <c r="P43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q43">
         <v>0.21915585000000001</v>
@@ -4760,7 +4760,7 @@
         <v>2050</v>
       </c>
       <c r="AB43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.3">
@@ -4768,10 +4768,10 @@
         <v>126</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D44">
         <v>10.005313230000001</v>
@@ -4810,7 +4810,7 @@
         <v>4.859685721</v>
       </c>
       <c r="P44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q44">
         <v>0.20577462399999999</v>
@@ -4846,7 +4846,7 @@
         <v>2050</v>
       </c>
       <c r="AB44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.3">
@@ -4854,10 +4854,10 @@
         <v>127</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D45">
         <v>11.428225319999999</v>
@@ -4896,7 +4896,7 @@
         <v>4.2400303609999996</v>
       </c>
       <c r="P45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q45">
         <v>0.235847368</v>
@@ -4937,10 +4937,10 @@
         <v>128</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D46">
         <v>10.661631079999999</v>
@@ -4979,7 +4979,7 @@
         <v>4.5937232459999997</v>
       </c>
       <c r="P46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q46">
         <v>0.21768834300000001</v>
@@ -5020,10 +5020,10 @@
         <v>129</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D47">
         <v>9.4238525580000001</v>
@@ -5062,7 +5062,7 @@
         <v>4.7222207980000004</v>
       </c>
       <c r="P47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q47">
         <v>0.21176476999999999</v>
@@ -5103,10 +5103,10 @@
         <v>130</v>
       </c>
       <c r="B48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D48">
         <v>11.379433130000001</v>
@@ -5145,7 +5145,7 @@
         <v>4.8470943379999998</v>
       </c>
       <c r="P48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q48">
         <v>0.20630916799999999</v>
@@ -5186,10 +5186,10 @@
         <v>131</v>
       </c>
       <c r="B49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D49">
         <v>11.359311440000001</v>
@@ -5228,7 +5228,7 @@
         <v>4.8013278650000002</v>
       </c>
       <c r="P49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q49">
         <v>0.208275716</v>
@@ -5264,7 +5264,7 @@
         <v>2050</v>
       </c>
       <c r="AB49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:28" x14ac:dyDescent="0.3">
@@ -5272,10 +5272,10 @@
         <v>144</v>
       </c>
       <c r="B50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D50">
         <v>12.93</v>
@@ -5314,7 +5314,7 @@
         <v>4.824626866</v>
       </c>
       <c r="P50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q50">
         <v>0.207269915</v>
@@ -5355,10 +5355,10 @@
         <v>145</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D51">
         <v>12.38</v>
@@ -5397,7 +5397,7 @@
         <v>5.4298245610000002</v>
       </c>
       <c r="P51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q51">
         <v>0.18416801299999999</v>
@@ -5438,10 +5438,10 @@
         <v>146</v>
       </c>
       <c r="B52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D52">
         <v>7.82</v>
@@ -5480,7 +5480,7 @@
         <v>5.75</v>
       </c>
       <c r="P52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q52">
         <v>0.17391304299999999</v>
@@ -5521,10 +5521,10 @@
         <v>147</v>
       </c>
       <c r="B53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D53">
         <v>13.1</v>
@@ -5563,7 +5563,7 @@
         <v>5.019157088</v>
       </c>
       <c r="P53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q53">
         <v>0.19923664099999999</v>
@@ -5604,10 +5604,10 @@
         <v>148</v>
       </c>
       <c r="B54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D54">
         <v>9.99</v>
@@ -5646,7 +5646,7 @@
         <v>4.6465116279999998</v>
       </c>
       <c r="P54" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q54">
         <v>0.21521521499999999</v>
@@ -5687,10 +5687,10 @@
         <v>156</v>
       </c>
       <c r="B55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C55" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D55">
         <v>4.54</v>
@@ -5729,7 +5729,7 @@
         <v>4.9397953729999999</v>
       </c>
       <c r="P55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q55">
         <v>0.202437535</v>
@@ -5770,10 +5770,10 @@
         <v>157</v>
       </c>
       <c r="B56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C56" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D56">
         <v>5.76</v>
@@ -5812,7 +5812,7 @@
         <v>5.459923034</v>
       </c>
       <c r="P56" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q56">
         <v>0.183152765</v>
@@ -5853,10 +5853,10 @@
         <v>158</v>
       </c>
       <c r="B57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D57">
         <v>7.96</v>
@@ -5895,7 +5895,7 @@
         <v>6.5433385609999997</v>
       </c>
       <c r="P57" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q57">
         <v>0.15282718300000001</v>
@@ -5936,10 +5936,10 @@
         <v>159</v>
       </c>
       <c r="B58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C58" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D58">
         <v>8.7899999999999991</v>
@@ -5978,7 +5978,7 @@
         <v>6.3829842990000003</v>
       </c>
       <c r="P58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q58">
         <v>0.15666653</v>
@@ -6019,10 +6019,10 @@
         <v>160</v>
       </c>
       <c r="B59" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D59">
         <v>6.53</v>
@@ -6061,7 +6061,7 @@
         <v>6.4642058330000003</v>
       </c>
       <c r="P59" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q59">
         <v>0.15469804400000001</v>
@@ -6102,10 +6102,10 @@
         <v>161</v>
       </c>
       <c r="B60" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C60" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D60">
         <v>6.56</v>
@@ -6144,7 +6144,7 @@
         <v>5.8028054850000004</v>
       </c>
       <c r="P60" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q60">
         <v>0.172330436</v>
@@ -6185,10 +6185,10 @@
         <v>162</v>
       </c>
       <c r="B61" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C61" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D61">
         <v>5.97</v>
@@ -6227,7 +6227,7 @@
         <v>5.4554112569999997</v>
       </c>
       <c r="P61" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q61">
         <v>0.18330423700000001</v>
@@ -6268,10 +6268,10 @@
         <v>163</v>
       </c>
       <c r="B62" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C62" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D62">
         <v>8.4700000000000006</v>
@@ -6310,7 +6310,7 @@
         <v>5.9409134479999999</v>
       </c>
       <c r="P62" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q62">
         <v>0.16832428399999999</v>
@@ -6351,10 +6351,10 @@
         <v>164</v>
       </c>
       <c r="B63" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C63" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D63">
         <v>7.06</v>
@@ -6393,7 +6393,7 @@
         <v>5.7314734639999996</v>
       </c>
       <c r="P63" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q63">
         <v>0.17447520399999999</v>
@@ -6434,10 +6434,10 @@
         <v>165</v>
       </c>
       <c r="B64" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D64">
         <v>8.6199999999999992</v>
@@ -6476,7 +6476,7 @@
         <v>5.5060444520000003</v>
       </c>
       <c r="P64" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q64">
         <v>0.181618585</v>
@@ -6517,10 +6517,10 @@
         <v>166</v>
       </c>
       <c r="B65" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C65" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D65">
         <v>8.09</v>
@@ -6559,7 +6559,7 @@
         <v>5.3740597660000002</v>
       </c>
       <c r="P65" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q65">
         <v>0.18607906199999999</v>
@@ -6600,10 +6600,10 @@
         <v>167</v>
       </c>
       <c r="B66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C66" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D66">
         <v>7.16</v>
@@ -6642,7 +6642,7 @@
         <v>7.3942341730000001</v>
       </c>
       <c r="P66" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q66">
         <v>0.13524051000000001</v>
@@ -6683,10 +6683,10 @@
         <v>168</v>
       </c>
       <c r="B67" t="s">
+        <v>105</v>
+      </c>
+      <c r="C67" t="s">
         <v>106</v>
-      </c>
-      <c r="C67" t="s">
-        <v>107</v>
       </c>
       <c r="D67">
         <v>9.9700000000000006</v>
@@ -6722,7 +6722,7 @@
         <v>7.9315831340000003</v>
       </c>
       <c r="P67" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q67">
         <v>0.12607823500000001</v>
@@ -6763,10 +6763,10 @@
         <v>169</v>
       </c>
       <c r="B68" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D68">
         <v>14.1</v>
@@ -6802,7 +6802,7 @@
         <v>7.0712136409999999</v>
       </c>
       <c r="P68" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q68">
         <v>0.14141844000000001</v>
@@ -6843,10 +6843,10 @@
         <v>170</v>
       </c>
       <c r="B69" t="s">
+        <v>108</v>
+      </c>
+      <c r="C69" t="s">
         <v>109</v>
-      </c>
-      <c r="C69" t="s">
-        <v>110</v>
       </c>
       <c r="D69">
         <v>16.62</v>
@@ -6882,7 +6882,7 @@
         <v>8.5980341439999997</v>
       </c>
       <c r="P69" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q69">
         <v>0.11630565599999999</v>
@@ -6923,10 +6923,10 @@
         <v>171</v>
       </c>
       <c r="B70" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C70" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D70">
         <v>15.73</v>
@@ -6962,7 +6962,7 @@
         <v>7.7794263109999999</v>
       </c>
       <c r="P70" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q70">
         <v>0.12854418300000001</v>

</xml_diff>